<commit_message>
Added MAGs produced in the study
</commit_message>
<xml_diff>
--- a/ModelGeneration_Files/D7SCFA_BioSampleIDs.xlsx
+++ b/ModelGeneration_Files/D7SCFA_BioSampleIDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irina/Desktop/Study/UofT/ParkinsonLab/Modeling_chickens/2023_ChickenCecalData_BenWilling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irina/Desktop/Study/UofT/ParkinsonLab/Modeling_chickens/Chicken_cecal_microbiome_project/ModelGeneration_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{46A5FFF9-B325-0449-AA9F-A4A252185E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2EB7A6B2-B83A-0247-BEE8-6F7624154DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="35840" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D7SCFA" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="314" uniqueCount="120">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="314" uniqueCount="121">
   <si>
     <t>A37-1</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>CopyNumber_per_g</t>
+  </si>
+  <si>
+    <t>NB</t>
   </si>
 </sst>
 </file>
@@ -934,7 +937,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
@@ -948,9 +951,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1310,7 +1311,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1395,8 +1396,8 @@
       <c r="I2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>67</v>
+      <c r="J2" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K2" t="s">
         <v>80</v>
@@ -1433,8 +1434,8 @@
       <c r="I3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>67</v>
+      <c r="J3" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K3" t="s">
         <v>80</v>
@@ -1471,8 +1472,8 @@
       <c r="I4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>67</v>
+      <c r="J4" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K4" t="s">
         <v>79</v>
@@ -1509,7 +1510,7 @@
       <c r="I5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K5" t="s">
@@ -1547,8 +1548,8 @@
       <c r="I6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="12" t="s">
-        <v>67</v>
+      <c r="J6" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K6" t="s">
         <v>80</v>
@@ -1585,7 +1586,7 @@
       <c r="I7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K7" t="s">
@@ -1623,8 +1624,8 @@
       <c r="I8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="12" t="s">
-        <v>67</v>
+      <c r="J8" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K8" t="s">
         <v>80</v>
@@ -1661,7 +1662,7 @@
       <c r="I9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K9" t="s">
@@ -1699,7 +1700,7 @@
       <c r="I10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K10" t="s">
@@ -1737,8 +1738,8 @@
       <c r="I11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>67</v>
+      <c r="J11" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K11" t="s">
         <v>80</v>
@@ -1775,7 +1776,7 @@
       <c r="I12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K12" t="s">
@@ -1785,41 +1786,41 @@
         <v>12194922373.393801</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13">
         <v>0.11486440000000001</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13">
         <v>1.4521344E-2</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13">
         <v>1.125607E-3</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13">
         <v>1.3370518E-2</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13">
         <v>1.611852E-3</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13">
         <v>2.8192320000000001E-3</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13">
         <v>0.148312953</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="11" t="s">
+      <c r="J13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" t="s">
         <v>80</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13">
         <v>12928706040.868299</v>
       </c>
     </row>
@@ -1851,8 +1852,8 @@
       <c r="I14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>67</v>
+      <c r="J14" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K14" t="s">
         <v>79</v>
@@ -1889,8 +1890,8 @@
       <c r="I15" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>67</v>
+      <c r="J15" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K15" t="s">
         <v>80</v>
@@ -1927,8 +1928,8 @@
       <c r="I16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>67</v>
+      <c r="J16" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K16" t="s">
         <v>79</v>
@@ -1965,7 +1966,7 @@
       <c r="I17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K17" t="s">
@@ -2003,7 +2004,7 @@
       <c r="I18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K18" t="s">
@@ -2041,8 +2042,8 @@
       <c r="I19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="12" t="s">
-        <v>67</v>
+      <c r="J19" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K19" t="s">
         <v>80</v>
@@ -2079,8 +2080,8 @@
       <c r="I20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J20" s="12" t="s">
-        <v>67</v>
+      <c r="J20" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K20" t="s">
         <v>80</v>
@@ -2117,7 +2118,7 @@
       <c r="I21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J21" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K21" t="s">
@@ -2155,7 +2156,7 @@
       <c r="I22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K22" t="s">
@@ -2193,7 +2194,7 @@
       <c r="I23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J23" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K23" t="s">
@@ -2231,8 +2232,8 @@
       <c r="I24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J24" s="12" t="s">
-        <v>67</v>
+      <c r="J24" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K24" t="s">
         <v>80</v>
@@ -2269,8 +2270,8 @@
       <c r="I25" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>67</v>
+      <c r="J25" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K25" t="s">
         <v>80</v>
@@ -2307,8 +2308,8 @@
       <c r="I26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="12" t="s">
-        <v>67</v>
+      <c r="J26" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K26" t="s">
         <v>79</v>
@@ -2345,8 +2346,8 @@
       <c r="I27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>67</v>
+      <c r="J27" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K27" t="s">
         <v>80</v>
@@ -2383,8 +2384,8 @@
       <c r="I28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="12" t="s">
-        <v>67</v>
+      <c r="J28" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K28" t="s">
         <v>79</v>
@@ -2421,7 +2422,7 @@
       <c r="I29" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="J29" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K29" t="s">
@@ -2459,7 +2460,7 @@
       <c r="I30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K30" t="s">
@@ -2498,7 +2499,7 @@
       <c r="I31" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J31" s="12" t="s">
+      <c r="J31" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K31" t="s">
@@ -2536,7 +2537,7 @@
       <c r="I32" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J32" s="12" t="s">
+      <c r="J32" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K32" t="s">
@@ -2574,7 +2575,7 @@
       <c r="I33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="11" t="s">
         <v>66</v>
       </c>
       <c r="K33" t="s">
@@ -2612,8 +2613,8 @@
       <c r="I34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J34" s="12" t="s">
-        <v>67</v>
+      <c r="J34" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="K34" t="s">
         <v>80</v>
@@ -3210,7 +3211,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C33"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>